<commit_message>
Updated Documentation on RTOS Threads
</commit_message>
<xml_diff>
--- a/Software/BatteryBalancer_Threads.xlsx
+++ b/Software/BatteryBalancer_Threads.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="42">
   <si>
     <t>Events</t>
   </si>
@@ -75,13 +75,88 @@
   </si>
   <si>
     <t>BatteryController</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Type </t>
+  </si>
+  <si>
+    <t>Func</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Thread</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Event_post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recieves output of posted I2C events </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recieves output of posted SPI events </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recieves output of posted I2C receive events </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Recieves output of posted StateChange events </t>
+  </si>
+  <si>
+    <t>SendCAN</t>
+  </si>
+  <si>
+    <t>Repeatadly calls sendCAN with a period of 500millisec and a timeoutof 1000millisec</t>
+  </si>
+  <si>
+    <t>SPI_HandleInterrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Timer_ISR </t>
+  </si>
+  <si>
+    <t>Increments timer</t>
+  </si>
+  <si>
+    <t>I2C_TCA9555Interupt</t>
+  </si>
+  <si>
+    <t>I2C_Interrupt</t>
+  </si>
+  <si>
+    <t>Sets state for new inputs from TCA9555 to True</t>
+  </si>
+  <si>
+    <t>Interrupt c2000 generates for when you are allowed to modify registers for I2C</t>
+  </si>
+  <si>
+    <t>CAN_Recieve_Interrupt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Checks for timeout /mailbox needs data to be read out of it | disables the mailbox once read from it  | Swaps mailbox message ID and re-enables it </t>
+  </si>
+  <si>
+    <t>SPI_HandleEvent</t>
+  </si>
+  <si>
+    <t>Processes pending SPI event, which is a transmition ready event and an spi done event</t>
+  </si>
+  <si>
+    <t>BatteryController_Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Task run forever | triggers I2c update | fetches state | checks THEN processes states | </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -96,6 +171,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -118,9 +198,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +479,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -477,6 +558,185 @@
         <v>14</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" t="s">
+        <v>41</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>